<commit_message>
added august based data filtering and 4h and 2h based resampling on that filter.
</commit_message>
<xml_diff>
--- a/Output_CSV/IF_anomaly.xlsx
+++ b/Output_CSV/IF_anomaly.xlsx
@@ -8,19 +8,56 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livemissouristate-my.sharepoint.com/personal/mt5864s_login_missouristate_edu/Documents/Documents/Jupyter Notebooks/Thesis/Output_CSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9ABF41E4-6711-4E12-9A27-D53C24B94EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{9ABF41E4-6711-4E12-9A27-D53C24B94EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DCED813-A796-4C1C-9D11-DBB43DB5CDDA}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{975C5AF7-7260-4222-883F-2C5673D8DC44}"/>
   </bookViews>
   <sheets>
     <sheet name="IF_anomaly" sheetId="1" r:id="rId1"/>
+    <sheet name="IF_anomaly_Aug" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={99A22AD5-300D-486B-A34E-413C914BEE8A}</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{99A22AD5-300D-486B-A34E-413C914BEE8A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    -1 for anomaly, 1 for regular</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={BF026224-4B4C-47F2-A644-D1D0B932BF0F}</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{BF026224-4B4C-47F2-A644-D1D0B932BF0F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    -1 for anomalies, 1 for regular data</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>datetime</t>
   </si>
@@ -35,7 +72,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +206,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -560,7 +603,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -579,6 +629,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Tanvir, Md Asif" id="{47E6851F-D003-48AA-BA94-3FED31046DEA}" userId="S::mt5864s@login.missouristate.edu::78dc76d4-91ef-4d65-9138-85e787734d21" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -896,12 +952,28 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C1" dT="2024-10-22T16:50:55.40" personId="{47E6851F-D003-48AA-BA94-3FED31046DEA}" id="{99A22AD5-300D-486B-A34E-413C914BEE8A}">
+    <text>-1 for anomaly, 1 for regular</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C1" dT="2024-10-22T16:48:55.02" personId="{47E6851F-D003-48AA-BA94-3FED31046DEA}" id="{BF026224-4B4C-47F2-A644-D1D0B932BF0F}">
+    <text>-1 for anomalies, 1 for regular data</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39CADF93-9DCC-41E4-9A8B-2EAD54FA34D4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39CADF93-9DCC-41E4-9A8B-2EAD54FA34D4}">
   <dimension ref="A1:C369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4971,10 +5043,2857 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>SEARCH(-1, $C1)&gt;0</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517ADB51-AFD9-4552-AA8E-F5A147DB6922}">
+  <dimension ref="A1:C255"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>45524.5</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45524.666666666664</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45524.833333333336</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45525</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45525.166666666664</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45525.333333333336</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45525.5</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45525.666666666664</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45525.833333333336</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45526</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45526.166666666664</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45526.333333333336</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45526.5</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45526.666666666664</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45526.833333333336</v>
+      </c>
+      <c r="B16">
+        <v>87</v>
+      </c>
+      <c r="C16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45527</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45527.166666666664</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45527.333333333336</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>45527.5</v>
+      </c>
+      <c r="B20">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>45527.666666666664</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>45527.833333333336</v>
+      </c>
+      <c r="B22">
+        <v>119</v>
+      </c>
+      <c r="C22">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>45528</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>45528.166666666664</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>45528.333333333336</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>45528.5</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>45528.666666666664</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>45528.833333333336</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>45529</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>45529.166666666664</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>45529.333333333336</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>45529.5</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>45529.666666666664</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>45529.833333333336</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>45530</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>45530.166666666664</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>45530.333333333336</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>45530.5</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>45530.666666666664</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>45530.833333333336</v>
+      </c>
+      <c r="B40">
+        <v>115</v>
+      </c>
+      <c r="C40">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>45531</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>45531.166666666664</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>45531.333333333336</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>45531.5</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>45531.666666666664</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>45531.833333333336</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>45532</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>45532.166666666664</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>45532.333333333336</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>45532.5</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>45532.666666666664</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>45532.833333333336</v>
+      </c>
+      <c r="B52">
+        <v>17</v>
+      </c>
+      <c r="C52">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>45533</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>45533.166666666664</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>45533.333333333336</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>45533.5</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>45533.666666666664</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>45533.833333333336</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>45534</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>45534.166666666664</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>45534.333333333336</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>45534.5</v>
+      </c>
+      <c r="B62">
+        <v>62</v>
+      </c>
+      <c r="C62">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>45534.666666666664</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>45534.833333333336</v>
+      </c>
+      <c r="B64">
+        <v>132</v>
+      </c>
+      <c r="C64">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>45535</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>45535.166666666664</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>45535.333333333336</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>45535.5</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>45535.666666666664</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>45535.833333333336</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>45536</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>45536.166666666664</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>45536.333333333336</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>45536.5</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>45536.666666666664</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>45536.833333333336</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>45537</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>45537.166666666664</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>45537.333333333336</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>45537.5</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>45537.666666666664</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>45537.833333333336</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>45538</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>45538.166666666664</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>45538.333333333336</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>45538.5</v>
+      </c>
+      <c r="B86">
+        <v>15</v>
+      </c>
+      <c r="C86">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>45538.666666666664</v>
+      </c>
+      <c r="B87">
+        <v>124</v>
+      </c>
+      <c r="C87">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>45538.833333333336</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>45539</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>45539.166666666664</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>45539.333333333336</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>45539.5</v>
+      </c>
+      <c r="B92">
+        <v>6</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>45539.666666666664</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>45539.833333333336</v>
+      </c>
+      <c r="B94">
+        <v>132</v>
+      </c>
+      <c r="C94">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>45540</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>45540.166666666664</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>45540.333333333336</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>45540.5</v>
+      </c>
+      <c r="B98">
+        <v>6</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>45540.666666666664</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>45540.833333333336</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>45541</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>45541.166666666664</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>45541.333333333336</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="C103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>45541.5</v>
+      </c>
+      <c r="B104">
+        <v>4</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>45541.666666666664</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>45541.833333333336</v>
+      </c>
+      <c r="B106">
+        <v>264</v>
+      </c>
+      <c r="C106">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>45542</v>
+      </c>
+      <c r="B107">
+        <v>32</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>45542.166666666664</v>
+      </c>
+      <c r="B108">
+        <v>30</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>45542.333333333336</v>
+      </c>
+      <c r="B109">
+        <v>37</v>
+      </c>
+      <c r="C109">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>45542.5</v>
+      </c>
+      <c r="B110">
+        <v>7</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>45542.666666666664</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>45542.833333333336</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>45543</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>45543.166666666664</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>45543.333333333336</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>45543.5</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>45543.666666666664</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>45543.833333333336</v>
+      </c>
+      <c r="B118">
+        <v>0</v>
+      </c>
+      <c r="C118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>45544</v>
+      </c>
+      <c r="B119">
+        <v>0</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>45544.166666666664</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>45544.333333333336</v>
+      </c>
+      <c r="B121">
+        <v>0</v>
+      </c>
+      <c r="C121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>45544.5</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>45544.666666666664</v>
+      </c>
+      <c r="B123">
+        <v>23</v>
+      </c>
+      <c r="C123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>45544.833333333336</v>
+      </c>
+      <c r="B124">
+        <v>31</v>
+      </c>
+      <c r="C124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>45545</v>
+      </c>
+      <c r="B125">
+        <v>22</v>
+      </c>
+      <c r="C125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>45545.166666666664</v>
+      </c>
+      <c r="B126">
+        <v>33</v>
+      </c>
+      <c r="C126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>45545.333333333336</v>
+      </c>
+      <c r="B127">
+        <v>35</v>
+      </c>
+      <c r="C127">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>45545.5</v>
+      </c>
+      <c r="B128">
+        <v>43</v>
+      </c>
+      <c r="C128">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>45545.666666666664</v>
+      </c>
+      <c r="B129">
+        <v>33</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>45545.833333333336</v>
+      </c>
+      <c r="B130">
+        <v>25</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>45546</v>
+      </c>
+      <c r="B131">
+        <v>28</v>
+      </c>
+      <c r="C131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>45546.166666666664</v>
+      </c>
+      <c r="B132">
+        <v>21</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>45546.333333333336</v>
+      </c>
+      <c r="B133">
+        <v>26</v>
+      </c>
+      <c r="C133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>45546.5</v>
+      </c>
+      <c r="B134">
+        <v>40</v>
+      </c>
+      <c r="C134">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>45546.666666666664</v>
+      </c>
+      <c r="B135">
+        <v>27</v>
+      </c>
+      <c r="C135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>45546.833333333336</v>
+      </c>
+      <c r="B136">
+        <v>293</v>
+      </c>
+      <c r="C136">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>45547</v>
+      </c>
+      <c r="B137">
+        <v>59</v>
+      </c>
+      <c r="C137">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>45547.166666666664</v>
+      </c>
+      <c r="B138">
+        <v>64</v>
+      </c>
+      <c r="C138">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>45547.333333333336</v>
+      </c>
+      <c r="B139">
+        <v>55</v>
+      </c>
+      <c r="C139">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>45547.5</v>
+      </c>
+      <c r="B140">
+        <v>60</v>
+      </c>
+      <c r="C140">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>45547.666666666664</v>
+      </c>
+      <c r="B141">
+        <v>49</v>
+      </c>
+      <c r="C141">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>45547.833333333336</v>
+      </c>
+      <c r="B142">
+        <v>65</v>
+      </c>
+      <c r="C142">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>45548</v>
+      </c>
+      <c r="B143">
+        <v>24</v>
+      </c>
+      <c r="C143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>45548.166666666664</v>
+      </c>
+      <c r="B144">
+        <v>37</v>
+      </c>
+      <c r="C144">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>45548.333333333336</v>
+      </c>
+      <c r="B145">
+        <v>29</v>
+      </c>
+      <c r="C145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>45548.5</v>
+      </c>
+      <c r="B146">
+        <v>44</v>
+      </c>
+      <c r="C146">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>45548.666666666664</v>
+      </c>
+      <c r="B147">
+        <v>27</v>
+      </c>
+      <c r="C147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>45548.833333333336</v>
+      </c>
+      <c r="B148">
+        <v>346</v>
+      </c>
+      <c r="C148">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>45549</v>
+      </c>
+      <c r="B149">
+        <v>29</v>
+      </c>
+      <c r="C149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>45549.166666666664</v>
+      </c>
+      <c r="B150">
+        <v>20</v>
+      </c>
+      <c r="C150">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>45549.333333333336</v>
+      </c>
+      <c r="B151">
+        <v>28</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>45549.5</v>
+      </c>
+      <c r="B152">
+        <v>26</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>45549.666666666664</v>
+      </c>
+      <c r="B153">
+        <v>26</v>
+      </c>
+      <c r="C153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>45549.833333333336</v>
+      </c>
+      <c r="B154">
+        <v>27</v>
+      </c>
+      <c r="C154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>45550</v>
+      </c>
+      <c r="B155">
+        <v>32</v>
+      </c>
+      <c r="C155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <v>45550.166666666664</v>
+      </c>
+      <c r="B156">
+        <v>28</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>45550.333333333336</v>
+      </c>
+      <c r="B157">
+        <v>25</v>
+      </c>
+      <c r="C157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>45550.5</v>
+      </c>
+      <c r="B158">
+        <v>24</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>45550.666666666664</v>
+      </c>
+      <c r="B159">
+        <v>424</v>
+      </c>
+      <c r="C159">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>45550.833333333336</v>
+      </c>
+      <c r="B160">
+        <v>573</v>
+      </c>
+      <c r="C160">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>45551</v>
+      </c>
+      <c r="B161">
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <v>45551.166666666664</v>
+      </c>
+      <c r="B162">
+        <v>1</v>
+      </c>
+      <c r="C162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <v>45551.333333333336</v>
+      </c>
+      <c r="B163">
+        <v>0</v>
+      </c>
+      <c r="C163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>45551.5</v>
+      </c>
+      <c r="B164">
+        <v>85</v>
+      </c>
+      <c r="C164">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <v>45551.666666666664</v>
+      </c>
+      <c r="B165">
+        <v>344</v>
+      </c>
+      <c r="C165">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>45551.833333333336</v>
+      </c>
+      <c r="B166">
+        <v>0</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>45552</v>
+      </c>
+      <c r="B167">
+        <v>0</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <v>45552.166666666664</v>
+      </c>
+      <c r="B168">
+        <v>0</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="1">
+        <v>45552.333333333336</v>
+      </c>
+      <c r="B169">
+        <v>0</v>
+      </c>
+      <c r="C169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="1">
+        <v>45552.5</v>
+      </c>
+      <c r="B170">
+        <v>8</v>
+      </c>
+      <c r="C170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="1">
+        <v>45552.666666666664</v>
+      </c>
+      <c r="B171">
+        <v>0</v>
+      </c>
+      <c r="C171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>45552.833333333336</v>
+      </c>
+      <c r="B172">
+        <v>37</v>
+      </c>
+      <c r="C172">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>45553</v>
+      </c>
+      <c r="B173">
+        <v>0</v>
+      </c>
+      <c r="C173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="1">
+        <v>45553.166666666664</v>
+      </c>
+      <c r="B174">
+        <v>0</v>
+      </c>
+      <c r="C174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="1">
+        <v>45553.333333333336</v>
+      </c>
+      <c r="B175">
+        <v>0</v>
+      </c>
+      <c r="C175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <v>45553.5</v>
+      </c>
+      <c r="B176">
+        <v>8</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>45553.666666666664</v>
+      </c>
+      <c r="B177">
+        <v>275</v>
+      </c>
+      <c r="C177">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <v>45553.833333333336</v>
+      </c>
+      <c r="B178">
+        <v>0</v>
+      </c>
+      <c r="C178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="1">
+        <v>45554</v>
+      </c>
+      <c r="B179">
+        <v>0</v>
+      </c>
+      <c r="C179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <v>45554.166666666664</v>
+      </c>
+      <c r="B180">
+        <v>0</v>
+      </c>
+      <c r="C180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="1">
+        <v>45554.333333333336</v>
+      </c>
+      <c r="B181">
+        <v>0</v>
+      </c>
+      <c r="C181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="1">
+        <v>45554.5</v>
+      </c>
+      <c r="B182">
+        <v>8</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <v>45554.666666666664</v>
+      </c>
+      <c r="B183">
+        <v>124</v>
+      </c>
+      <c r="C183">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>45554.833333333336</v>
+      </c>
+      <c r="B184">
+        <v>0</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>45555</v>
+      </c>
+      <c r="B185">
+        <v>0</v>
+      </c>
+      <c r="C185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>45555.166666666664</v>
+      </c>
+      <c r="B186">
+        <v>0</v>
+      </c>
+      <c r="C186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>45555.333333333336</v>
+      </c>
+      <c r="B187">
+        <v>0</v>
+      </c>
+      <c r="C187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>45555.5</v>
+      </c>
+      <c r="B188">
+        <v>13</v>
+      </c>
+      <c r="C188">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>45555.666666666664</v>
+      </c>
+      <c r="B189">
+        <v>0</v>
+      </c>
+      <c r="C189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>45555.833333333336</v>
+      </c>
+      <c r="B190">
+        <v>325</v>
+      </c>
+      <c r="C190">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>45556</v>
+      </c>
+      <c r="B191">
+        <v>0</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>45556.166666666664</v>
+      </c>
+      <c r="B192">
+        <v>0</v>
+      </c>
+      <c r="C192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>45556.333333333336</v>
+      </c>
+      <c r="B193">
+        <v>0</v>
+      </c>
+      <c r="C193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>45556.5</v>
+      </c>
+      <c r="B194">
+        <v>0</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>45556.666666666664</v>
+      </c>
+      <c r="B195">
+        <v>0</v>
+      </c>
+      <c r="C195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>45556.833333333336</v>
+      </c>
+      <c r="B196">
+        <v>0</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>45557</v>
+      </c>
+      <c r="B197">
+        <v>0</v>
+      </c>
+      <c r="C197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>45557.166666666664</v>
+      </c>
+      <c r="B198">
+        <v>0</v>
+      </c>
+      <c r="C198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>45557.333333333336</v>
+      </c>
+      <c r="B199">
+        <v>0</v>
+      </c>
+      <c r="C199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>45557.5</v>
+      </c>
+      <c r="B200">
+        <v>0</v>
+      </c>
+      <c r="C200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
+        <v>45557.666666666664</v>
+      </c>
+      <c r="B201">
+        <v>0</v>
+      </c>
+      <c r="C201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
+        <v>45557.833333333336</v>
+      </c>
+      <c r="B202">
+        <v>0</v>
+      </c>
+      <c r="C202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>45558</v>
+      </c>
+      <c r="B203">
+        <v>0</v>
+      </c>
+      <c r="C203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
+        <v>45558.166666666664</v>
+      </c>
+      <c r="B204">
+        <v>0</v>
+      </c>
+      <c r="C204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>45558.333333333336</v>
+      </c>
+      <c r="B205">
+        <v>0</v>
+      </c>
+      <c r="C205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
+        <v>45558.5</v>
+      </c>
+      <c r="B206">
+        <v>0</v>
+      </c>
+      <c r="C206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>45558.666666666664</v>
+      </c>
+      <c r="B207">
+        <v>0</v>
+      </c>
+      <c r="C207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>45558.833333333336</v>
+      </c>
+      <c r="B208">
+        <v>0</v>
+      </c>
+      <c r="C208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="1">
+        <v>45559</v>
+      </c>
+      <c r="B209">
+        <v>0</v>
+      </c>
+      <c r="C209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="1">
+        <v>45559.166666666664</v>
+      </c>
+      <c r="B210">
+        <v>0</v>
+      </c>
+      <c r="C210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="1">
+        <v>45559.333333333336</v>
+      </c>
+      <c r="B211">
+        <v>0</v>
+      </c>
+      <c r="C211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="1">
+        <v>45559.5</v>
+      </c>
+      <c r="B212">
+        <v>7</v>
+      </c>
+      <c r="C212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="1">
+        <v>45559.666666666664</v>
+      </c>
+      <c r="B213">
+        <v>0</v>
+      </c>
+      <c r="C213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="1">
+        <v>45559.833333333336</v>
+      </c>
+      <c r="B214">
+        <v>35</v>
+      </c>
+      <c r="C214">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="1">
+        <v>45560</v>
+      </c>
+      <c r="B215">
+        <v>0</v>
+      </c>
+      <c r="C215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="1">
+        <v>45560.166666666664</v>
+      </c>
+      <c r="B216">
+        <v>0</v>
+      </c>
+      <c r="C216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" s="1">
+        <v>45560.333333333336</v>
+      </c>
+      <c r="B217">
+        <v>0</v>
+      </c>
+      <c r="C217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="1">
+        <v>45560.5</v>
+      </c>
+      <c r="B218">
+        <v>8</v>
+      </c>
+      <c r="C218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" s="1">
+        <v>45560.666666666664</v>
+      </c>
+      <c r="B219">
+        <v>0</v>
+      </c>
+      <c r="C219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="1">
+        <v>45560.833333333336</v>
+      </c>
+      <c r="B220">
+        <v>0</v>
+      </c>
+      <c r="C220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" s="1">
+        <v>45561</v>
+      </c>
+      <c r="B221">
+        <v>0</v>
+      </c>
+      <c r="C221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="1">
+        <v>45561.166666666664</v>
+      </c>
+      <c r="B222">
+        <v>0</v>
+      </c>
+      <c r="C222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" s="1">
+        <v>45561.333333333336</v>
+      </c>
+      <c r="B223">
+        <v>0</v>
+      </c>
+      <c r="C223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="1">
+        <v>45561.5</v>
+      </c>
+      <c r="B224">
+        <v>7</v>
+      </c>
+      <c r="C224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" s="1">
+        <v>45561.666666666664</v>
+      </c>
+      <c r="B225">
+        <v>0</v>
+      </c>
+      <c r="C225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="1">
+        <v>45561.833333333336</v>
+      </c>
+      <c r="B226">
+        <v>0</v>
+      </c>
+      <c r="C226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="1">
+        <v>45562</v>
+      </c>
+      <c r="B227">
+        <v>0</v>
+      </c>
+      <c r="C227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="1">
+        <v>45562.166666666664</v>
+      </c>
+      <c r="B228">
+        <v>0</v>
+      </c>
+      <c r="C228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="1">
+        <v>45562.333333333336</v>
+      </c>
+      <c r="B229">
+        <v>0</v>
+      </c>
+      <c r="C229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="1">
+        <v>45562.5</v>
+      </c>
+      <c r="B230">
+        <v>7</v>
+      </c>
+      <c r="C230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="1">
+        <v>45562.666666666664</v>
+      </c>
+      <c r="B231">
+        <v>1</v>
+      </c>
+      <c r="C231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="1">
+        <v>45562.833333333336</v>
+      </c>
+      <c r="B232">
+        <v>214</v>
+      </c>
+      <c r="C232">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" s="1">
+        <v>45563</v>
+      </c>
+      <c r="B233">
+        <v>0</v>
+      </c>
+      <c r="C233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" s="1">
+        <v>45563.166666666664</v>
+      </c>
+      <c r="B234">
+        <v>0</v>
+      </c>
+      <c r="C234">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="1">
+        <v>45563.333333333336</v>
+      </c>
+      <c r="B235">
+        <v>0</v>
+      </c>
+      <c r="C235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="1">
+        <v>45563.5</v>
+      </c>
+      <c r="B236">
+        <v>0</v>
+      </c>
+      <c r="C236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="1">
+        <v>45563.666666666664</v>
+      </c>
+      <c r="B237">
+        <v>0</v>
+      </c>
+      <c r="C237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="1">
+        <v>45563.833333333336</v>
+      </c>
+      <c r="B238">
+        <v>1</v>
+      </c>
+      <c r="C238">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" s="1">
+        <v>45564</v>
+      </c>
+      <c r="B239">
+        <v>0</v>
+      </c>
+      <c r="C239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="1">
+        <v>45564.166666666664</v>
+      </c>
+      <c r="B240">
+        <v>1</v>
+      </c>
+      <c r="C240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="1">
+        <v>45564.333333333336</v>
+      </c>
+      <c r="B241">
+        <v>0</v>
+      </c>
+      <c r="C241">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="1">
+        <v>45564.5</v>
+      </c>
+      <c r="B242">
+        <v>0</v>
+      </c>
+      <c r="C242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="1">
+        <v>45564.666666666664</v>
+      </c>
+      <c r="B243">
+        <v>0</v>
+      </c>
+      <c r="C243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="1">
+        <v>45564.833333333336</v>
+      </c>
+      <c r="B244">
+        <v>0</v>
+      </c>
+      <c r="C244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" s="1">
+        <v>45565</v>
+      </c>
+      <c r="B245">
+        <v>0</v>
+      </c>
+      <c r="C245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" s="1">
+        <v>45565.166666666664</v>
+      </c>
+      <c r="B246">
+        <v>0</v>
+      </c>
+      <c r="C246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" s="1">
+        <v>45565.333333333336</v>
+      </c>
+      <c r="B247">
+        <v>0</v>
+      </c>
+      <c r="C247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" s="1">
+        <v>45565.5</v>
+      </c>
+      <c r="B248">
+        <v>9</v>
+      </c>
+      <c r="C248">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" s="1">
+        <v>45565.666666666664</v>
+      </c>
+      <c r="B249">
+        <v>0</v>
+      </c>
+      <c r="C249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" s="1">
+        <v>45565.833333333336</v>
+      </c>
+      <c r="B250">
+        <v>0</v>
+      </c>
+      <c r="C250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" s="1">
+        <v>45566</v>
+      </c>
+      <c r="B251">
+        <v>0</v>
+      </c>
+      <c r="C251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" s="1">
+        <v>45566.166666666664</v>
+      </c>
+      <c r="B252">
+        <v>0</v>
+      </c>
+      <c r="C252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" s="1">
+        <v>45566.333333333336</v>
+      </c>
+      <c r="B253">
+        <v>0</v>
+      </c>
+      <c r="C253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" s="1">
+        <v>45566.5</v>
+      </c>
+      <c r="B254">
+        <v>5</v>
+      </c>
+      <c r="C254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" s="1">
+        <v>45566.666666666664</v>
+      </c>
+      <c r="B255">
+        <v>335</v>
+      </c>
+      <c r="C255">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>